<commit_message>
ajuste en la carga de datos
</commit_message>
<xml_diff>
--- a/data/registro_entrega.xlsx
+++ b/data/registro_entrega.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,56 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>16:36:47</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>VIERNES</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>INVESTIGACIÓN CONTABLE</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>M-401</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>MICHAEL  GONZALEZ PULGARIN</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1036941224</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>18:00 a 19:00</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Entregada</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>